<commit_message>
con phan đồ thị vs excel
</commit_message>
<xml_diff>
--- a/Đo_An/HoanThanhDangNhap/bin/Debug/Resources2/Du lieu cau hoi/thu vien comp.xlsx
+++ b/Đo_An/HoanThanhDangNhap/bin/Debug/Resources2/Du lieu cau hoi/thu vien comp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Đồ Án\DO AN\Do_AN\TruaNgay18New1\student_add bai hoc\HoanThanhDangNhap\bin\Debug\Resources\Du lieu cau hoi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lam do an\Qua trinh CODE C#\DangHoanThien2504\student_add bai hoc_ 0904\student_add bai hoc\HoanThanhDangNhap\bin\Debug\Resources\Du lieu cau hoi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D204BEEB-193B-422B-B861-7CCE074A3303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E601A6-5964-4CF3-B82E-9C3998663D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{44CE0958-A6C1-42E6-8D55-7FA2B2385169}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{44CE0958-A6C1-42E6-8D55-7FA2B2385169}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D2A3BD-74E5-49D8-B5E0-F6FA57BFF832}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1025,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50800CD1-DAB9-4106-B762-75BC323C9169}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>